<commit_message>
Accounting Excel and BUS003
</commit_message>
<xml_diff>
--- a/ACCT_152/Chap 8 Royal Company class case  Excel Master Budget input sheet to generate master budget  3-25-23.xlsx
+++ b/ACCT_152/Chap 8 Royal Company class case  Excel Master Budget input sheet to generate master budget  3-25-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lbw/Documents/GitHub/fall_2023/ACCT_152/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FA9B18-5816-BB47-BE22-2E4A4EE13D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C4817E-184C-6246-B1D4-B55280C335C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,7 +548,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -559,6 +559,7 @@
     <numFmt numFmtId="168" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="169" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -677,7 +678,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -886,14 +887,17 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1615,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1635,12 +1639,12 @@
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1845,7 +1849,9 @@
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="15">
+        <v>0.5</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -1856,7 +1862,9 @@
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="15">
+        <v>0.5</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1867,7 +1875,9 @@
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="11">
+        <v>12000</v>
+      </c>
       <c r="C21" s="20"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1876,7 +1886,9 @@
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="21">
+        <v>0.05</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1887,7 +1899,9 @@
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="11">
+        <v>10</v>
+      </c>
       <c r="C23" s="20"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1896,7 +1910,9 @@
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="22"/>
+      <c r="B24" s="22">
+        <v>40</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1918,7 +1934,9 @@
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="11">
+        <v>20</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
@@ -1929,7 +1947,9 @@
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="11">
+        <v>30000</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1940,7 +1960,9 @@
       <c r="A28" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="11">
+        <v>20000</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>37</v>
       </c>
@@ -1951,7 +1973,10 @@
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="18">
+        <f>E105/SUM(B101:D101)</f>
+        <v>49.702970297029701</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1962,7 +1987,9 @@
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="23">
+        <v>0.5</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>41</v>
       </c>
@@ -1973,7 +2000,9 @@
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="11"/>
+      <c r="B31" s="11">
+        <v>60000</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1984,7 +2013,9 @@
       <c r="A32" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="11"/>
+      <c r="B32" s="11">
+        <v>10000</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1995,7 +2026,9 @@
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="11"/>
+      <c r="B33" s="11">
+        <v>30000</v>
+      </c>
       <c r="C33" s="1"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2004,7 +2037,9 @@
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="11"/>
+      <c r="B34" s="11">
+        <v>49000</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2013,7 +2048,9 @@
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="11">
+        <v>40000</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2022,7 +2059,9 @@
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="11"/>
+      <c r="B36" s="11">
+        <v>143700</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>47</v>
       </c>
@@ -2033,7 +2072,9 @@
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="11"/>
+      <c r="B37" s="11">
+        <v>48300</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>47</v>
       </c>
@@ -2044,7 +2085,9 @@
       <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="11"/>
+      <c r="B38" s="11">
+        <v>75000</v>
+      </c>
       <c r="C38" s="1"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2053,7 +2096,9 @@
       <c r="A39" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="13">
+        <v>0.16</v>
+      </c>
       <c r="C39" s="1"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2062,7 +2107,9 @@
       <c r="A40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="11"/>
+      <c r="B40" s="11">
+        <v>50000</v>
+      </c>
       <c r="C40" s="1"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2071,7 +2118,9 @@
       <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="11"/>
+      <c r="B41" s="11">
+        <v>150000</v>
+      </c>
       <c r="C41" s="1"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2080,7 +2129,9 @@
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="11"/>
+      <c r="B42" s="11">
+        <v>248650</v>
+      </c>
       <c r="C42" s="1"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2089,7 +2140,9 @@
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="11">
+        <v>175000</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2121,12 +2174,12 @@
       <c r="A47" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
     </row>
     <row r="48" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
@@ -2217,12 +2270,12 @@
       <c r="A53" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="72" t="s">
+      <c r="B53" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="72"/>
+      <c r="C53" s="70"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="70"/>
     </row>
     <row r="54" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
@@ -2337,12 +2390,12 @@
       <c r="A61" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="72"/>
+      <c r="C61" s="70"/>
+      <c r="D61" s="70"/>
+      <c r="E61" s="70"/>
     </row>
     <row r="62" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
@@ -2448,7 +2501,7 @@
         <v>69</v>
       </c>
       <c r="B67" s="36">
-        <f t="shared" ref="B67:E67" si="3">B65-B66</f>
+        <f t="shared" ref="B67:D67" si="3">B65-B66</f>
         <v>26000</v>
       </c>
       <c r="C67" s="36">
@@ -2475,12 +2528,12 @@
       <c r="A69" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="72" t="s">
+      <c r="B69" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="70"/>
     </row>
     <row r="70" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
@@ -2502,7 +2555,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="34">
-        <f t="shared" ref="B71:E71" si="4">B67</f>
+        <f t="shared" ref="B71:D71" si="4">B67</f>
         <v>26000</v>
       </c>
       <c r="C71" s="34">
@@ -2697,12 +2750,12 @@
       <c r="A81" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="72" t="s">
+      <c r="B81" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="72"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="72"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="70"/>
     </row>
     <row r="82" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
@@ -2725,13 +2778,13 @@
       </c>
       <c r="B83" s="31">
         <f>B21</f>
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="C83" s="31"/>
       <c r="D83" s="31"/>
       <c r="E83" s="42">
         <f>SUM(B83:D83)</f>
-        <v>0</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2740,16 +2793,16 @@
       </c>
       <c r="B84" s="32">
         <f>B79*B19</f>
-        <v>0</v>
+        <v>28000</v>
       </c>
       <c r="C84" s="31">
         <f>B79*B20</f>
-        <v>0</v>
+        <v>28000</v>
       </c>
       <c r="D84" s="31"/>
       <c r="E84" s="42">
         <f t="shared" ref="E84:E86" si="6">SUM(B84:D84)</f>
-        <v>0</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2759,15 +2812,15 @@
       <c r="B85" s="31"/>
       <c r="C85" s="32">
         <f>C79*B19</f>
-        <v>0</v>
+        <v>44300</v>
       </c>
       <c r="D85" s="31">
         <f>C79*B20</f>
-        <v>0</v>
+        <v>44300</v>
       </c>
       <c r="E85" s="42">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>88600</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2778,11 +2831,11 @@
       <c r="C86" s="31"/>
       <c r="D86" s="32">
         <f>D79*B19</f>
-        <v>0</v>
+        <v>28400</v>
       </c>
       <c r="E86" s="42">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>28400</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2791,19 +2844,19 @@
       </c>
       <c r="B87" s="29">
         <f>SUM(B83:B86)</f>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="C87" s="29">
         <f>SUM(C83:C86)</f>
-        <v>0</v>
+        <v>72300</v>
       </c>
       <c r="D87" s="29">
         <f>SUM(D83:D86)</f>
-        <v>0</v>
+        <v>72700</v>
       </c>
       <c r="E87" s="40">
         <f>SUM(E83:E86)</f>
-        <v>0</v>
+        <v>185000</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2817,12 +2870,12 @@
       <c r="A89" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B89" s="72" t="s">
+      <c r="B89" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C89" s="72"/>
-      <c r="D89" s="72"/>
-      <c r="E89" s="72"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="70"/>
+      <c r="E89" s="70"/>
     </row>
     <row r="90" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
@@ -2843,19 +2896,19 @@
       <c r="A91" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B91" s="24">
+      <c r="B91" s="73">
         <f>B71</f>
         <v>26000</v>
       </c>
-      <c r="C91" s="24">
-        <f t="shared" ref="C91:E91" si="7">C71</f>
+      <c r="C91" s="73">
+        <f t="shared" ref="C91:D91" si="7">C71</f>
         <v>46000</v>
       </c>
-      <c r="D91" s="24">
+      <c r="D91" s="73">
         <f t="shared" si="7"/>
         <v>29000</v>
       </c>
-      <c r="E91" s="24">
+      <c r="E91" s="73">
         <f>E71</f>
         <v>101000</v>
       </c>
@@ -2866,19 +2919,19 @@
       </c>
       <c r="B92" s="44">
         <f>$B$22</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C92" s="44">
         <f t="shared" ref="C92:E92" si="8">$B$22</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D92" s="44">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E92" s="44">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2887,19 +2940,19 @@
       </c>
       <c r="B93" s="8">
         <f>B91*B92</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="C93" s="8">
         <f t="shared" ref="C93:D93" si="9">C91*C92</f>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="D93" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1450</v>
       </c>
       <c r="E93" s="45">
         <f>E91*E92</f>
-        <v>0</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2926,19 +2979,19 @@
       </c>
       <c r="B95" s="8">
         <f>IF(B93&gt;B94,B93,B94)</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="C95" s="8">
         <f t="shared" ref="C95:D95" si="11">IF(C93&gt;C94,C93,C94)</f>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="D95" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1450</v>
       </c>
       <c r="E95" s="7">
         <f>SUM(B95:D95)</f>
-        <v>0</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,19 +3000,19 @@
       </c>
       <c r="B96" s="48">
         <f>$B$23</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C96" s="48">
         <f t="shared" ref="C96:E96" si="12">$B$23</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D96" s="48">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E96" s="48">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2968,19 +3021,19 @@
       </c>
       <c r="B97" s="49">
         <f>B95*B96</f>
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="C97" s="49">
         <f t="shared" ref="C97:E97" si="13">C95*C96</f>
-        <v>0</v>
+        <v>23000</v>
       </c>
       <c r="D97" s="49">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>14500</v>
       </c>
       <c r="E97" s="49">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>50500</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2994,12 +3047,12 @@
       <c r="A99" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B99" s="72" t="s">
+      <c r="B99" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="72"/>
-      <c r="D99" s="72"/>
-      <c r="E99" s="72"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="70"/>
+      <c r="E99" s="70"/>
     </row>
     <row r="100" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
@@ -3022,19 +3075,19 @@
       </c>
       <c r="B101" s="34">
         <f>B93</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="C101" s="34">
         <f t="shared" ref="C101:E101" si="14">C93</f>
-        <v>0</v>
+        <v>2300</v>
       </c>
       <c r="D101" s="34">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1450</v>
       </c>
       <c r="E101" s="34">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3043,19 +3096,19 @@
       </c>
       <c r="B102" s="48">
         <f>$B$26</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C102" s="48">
         <f t="shared" ref="C102:E102" si="15">$B$26</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D102" s="48">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E102" s="48">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3064,19 +3117,19 @@
       </c>
       <c r="B103" s="24">
         <f>B101*B102</f>
-        <v>0</v>
+        <v>26000</v>
       </c>
       <c r="C103" s="24">
         <f t="shared" ref="C103:E103" si="16">C101*C102</f>
-        <v>0</v>
+        <v>46000</v>
       </c>
       <c r="D103" s="24">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>29000</v>
       </c>
       <c r="E103" s="24">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>101000</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3085,19 +3138,19 @@
       </c>
       <c r="B104" s="48">
         <f>($B$27+$B$28)</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C104" s="48">
         <f t="shared" ref="C104:D104" si="17">($B$27+$B$28)</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D104" s="48">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="E104" s="48">
         <f>SUM(B104:D104)</f>
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3106,19 +3159,19 @@
       </c>
       <c r="B105" s="24">
         <f>B104+B103</f>
-        <v>0</v>
+        <v>76000</v>
       </c>
       <c r="C105" s="24">
         <f t="shared" ref="C105:E105" si="18">C104+C103</f>
-        <v>0</v>
+        <v>96000</v>
       </c>
       <c r="D105" s="24">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f>D104+D103</f>
+        <v>79000</v>
       </c>
       <c r="E105" s="24">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f>E104+E103</f>
+        <v>251000</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3127,19 +3180,19 @@
       </c>
       <c r="B106" s="48">
         <f>$B$28</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="C106" s="48">
         <f t="shared" ref="C106:D106" si="19">$B$28</f>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D106" s="48">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="E106" s="50">
         <f>SUM(B106:D106)</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3148,19 +3201,19 @@
       </c>
       <c r="B107" s="29">
         <f>B105-B106</f>
-        <v>0</v>
+        <v>56000</v>
       </c>
       <c r="C107" s="29">
         <f t="shared" ref="C107:E107" si="20">C105-C106</f>
-        <v>0</v>
+        <v>76000</v>
       </c>
       <c r="D107" s="29">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="E107" s="29">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>191000</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -3225,15 +3278,15 @@
       </c>
       <c r="B113" s="52">
         <f>B22</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C113" s="11">
         <f>B23</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D113" s="18">
         <f t="shared" ref="D113:D114" si="21">B113*C113</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E113" s="4"/>
     </row>
@@ -3243,15 +3296,15 @@
       </c>
       <c r="B114" s="44">
         <f>B22</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C114" s="53">
         <f>B29</f>
-        <v>0</v>
+        <v>49.702970297029701</v>
       </c>
       <c r="D114" s="53">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.4851485148514851</v>
       </c>
       <c r="E114" s="4"/>
     </row>
@@ -3261,7 +3314,7 @@
       <c r="C115" s="4"/>
       <c r="D115" s="54">
         <f>SUM(D112:D114)</f>
-        <v>2</v>
+        <v>4.9851485148514847</v>
       </c>
       <c r="E115" s="4"/>
     </row>
@@ -3294,7 +3347,7 @@
       <c r="C118" s="4"/>
       <c r="D118" s="55">
         <f>ROUND(D115,2)</f>
-        <v>2</v>
+        <v>4.99</v>
       </c>
       <c r="E118" s="4"/>
     </row>
@@ -3306,7 +3359,7 @@
       <c r="C119" s="4"/>
       <c r="D119" s="56">
         <f>D117*D118</f>
-        <v>10000</v>
+        <v>24950</v>
       </c>
       <c r="E119" s="4"/>
     </row>
@@ -3321,12 +3374,12 @@
       <c r="A121" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B121" s="72" t="s">
+      <c r="B121" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C121" s="72"/>
-      <c r="D121" s="72"/>
-      <c r="E121" s="72"/>
+      <c r="C121" s="70"/>
+      <c r="D121" s="70"/>
+      <c r="E121" s="70"/>
     </row>
     <row r="122" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
@@ -3370,19 +3423,19 @@
       </c>
       <c r="B124" s="57">
         <f>$B$30</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C124" s="57">
         <f t="shared" ref="C124:E124" si="23">$B$30</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D124" s="57">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E124" s="57">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3391,19 +3444,19 @@
       </c>
       <c r="B125" s="58">
         <f>B123*B124</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="C125" s="58">
         <f t="shared" ref="C125:E125" si="24">C123*C124</f>
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="D125" s="58">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E125" s="58">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3412,19 +3465,19 @@
       </c>
       <c r="B126" s="48">
         <f>($B$31+$B$32)</f>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="C126" s="48">
         <f t="shared" ref="C126:D126" si="25">($B$31+$B$32)</f>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="D126" s="48">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="E126" s="50">
         <f>SUM(B126:D126)</f>
-        <v>0</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3433,19 +3486,19 @@
       </c>
       <c r="B127" s="58">
         <f>B125+B126</f>
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="C127" s="58">
         <f t="shared" ref="C127:E127" si="26">C125+C126</f>
-        <v>0</v>
+        <v>95000</v>
       </c>
       <c r="D127" s="58">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>85000</v>
       </c>
       <c r="E127" s="58">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>260000</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3454,19 +3507,19 @@
       </c>
       <c r="B128" s="48">
         <f>$B$32</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="C128" s="48">
         <f t="shared" ref="C128:D128" si="27">$B$32</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D128" s="48">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E128" s="48">
         <f>SUM(B128:D128)</f>
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3475,19 +3528,19 @@
       </c>
       <c r="B129" s="29">
         <f>B127-B128</f>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="C129" s="29">
         <f t="shared" ref="C129:E129" si="28">C127-C128</f>
-        <v>0</v>
+        <v>85000</v>
       </c>
       <c r="D129" s="29">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="E129" s="29">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>230000</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -3501,12 +3554,12 @@
       <c r="A131" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B131" s="72" t="s">
+      <c r="B131" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C131" s="72"/>
-      <c r="D131" s="72"/>
-      <c r="E131" s="72"/>
+      <c r="C131" s="70"/>
+      <c r="D131" s="70"/>
+      <c r="E131" s="70"/>
     </row>
     <row r="132" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
@@ -3529,19 +3582,19 @@
       </c>
       <c r="B133" s="59">
         <f>B35</f>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="C133" s="43">
         <f>B150</f>
-        <v>170000</v>
+        <v>30000</v>
       </c>
       <c r="D133" s="4">
         <f>C150</f>
-        <v>580000</v>
+        <v>40000</v>
       </c>
       <c r="E133" s="60">
         <f>B133</f>
-        <v>0</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3571,19 +3624,19 @@
       </c>
       <c r="B135" s="62">
         <f>B134+B133</f>
-        <v>170000</v>
+        <v>210000</v>
       </c>
       <c r="C135" s="62">
         <f t="shared" ref="C135:E135" si="30">C134+C133</f>
-        <v>580000</v>
+        <v>440000</v>
       </c>
       <c r="D135" s="62">
         <f t="shared" si="30"/>
-        <v>940000</v>
+        <v>400000</v>
       </c>
       <c r="E135" s="62">
         <f t="shared" si="30"/>
-        <v>940000</v>
+        <v>980000</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3601,19 +3654,19 @@
       </c>
       <c r="B137" s="42">
         <f>B87</f>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="C137" s="42">
         <f t="shared" ref="C137:E137" si="31">C87</f>
-        <v>0</v>
+        <v>72300</v>
       </c>
       <c r="D137" s="42">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>72700</v>
       </c>
       <c r="E137" s="42">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>185000</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3622,19 +3675,19 @@
       </c>
       <c r="B138" s="42">
         <f>B97</f>
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="C138" s="42">
         <f t="shared" ref="C138:E138" si="32">C97</f>
-        <v>0</v>
+        <v>23000</v>
       </c>
       <c r="D138" s="42">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>14500</v>
       </c>
       <c r="E138" s="42">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>50500</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3643,19 +3696,19 @@
       </c>
       <c r="B139" s="42">
         <f>B107</f>
-        <v>0</v>
+        <v>56000</v>
       </c>
       <c r="C139" s="42">
         <f t="shared" ref="C139:E139" si="33">C107</f>
-        <v>0</v>
+        <v>76000</v>
       </c>
       <c r="D139" s="42">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="E139" s="42">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>191000</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3664,19 +3717,19 @@
       </c>
       <c r="B140" s="42">
         <f>B129</f>
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="C140" s="42">
         <f t="shared" ref="C140:E140" si="34">C129</f>
-        <v>0</v>
+        <v>85000</v>
       </c>
       <c r="D140" s="42">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>75000</v>
       </c>
       <c r="E140" s="42">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>230000</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3688,15 +3741,15 @@
       </c>
       <c r="C141" s="64">
         <f>B36</f>
-        <v>0</v>
+        <v>143700</v>
       </c>
       <c r="D141" s="64">
         <f>B37</f>
-        <v>0</v>
+        <v>48300</v>
       </c>
       <c r="E141" s="64">
         <f>SUM(B141:D141)</f>
-        <v>0</v>
+        <v>192000</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3705,7 +3758,7 @@
       </c>
       <c r="B142" s="42">
         <f>B34</f>
-        <v>0</v>
+        <v>49000</v>
       </c>
       <c r="C142" s="65">
         <v>0</v>
@@ -3715,7 +3768,7 @@
       </c>
       <c r="E142" s="64">
         <f>SUM(B142:D142)</f>
-        <v>0</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3724,19 +3777,19 @@
       </c>
       <c r="B143" s="66">
         <f>SUM(B137:B142)</f>
-        <v>0</v>
+        <v>228000</v>
       </c>
       <c r="C143" s="66">
-        <f t="shared" ref="C143:E143" si="35">SUM(C137:C142)</f>
-        <v>0</v>
+        <f>SUM(C137:C142)</f>
+        <v>400000</v>
       </c>
       <c r="D143" s="66">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <f t="shared" ref="C143:E143" si="35">SUM(D137:D142)</f>
+        <v>269500</v>
       </c>
       <c r="E143" s="67">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>897500</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3745,19 +3798,19 @@
       </c>
       <c r="B144" s="31">
         <f>B135-B143</f>
-        <v>170000</v>
+        <v>-18000</v>
       </c>
       <c r="C144" s="31">
-        <f t="shared" ref="C144:E144" si="36">C135-C143</f>
-        <v>580000</v>
+        <f>C135-C143</f>
+        <v>40000</v>
       </c>
       <c r="D144" s="31">
-        <f t="shared" si="36"/>
-        <v>940000</v>
+        <f t="shared" ref="C144:E144" si="36">D135-D143</f>
+        <v>130500</v>
       </c>
       <c r="E144" s="31">
         <f t="shared" si="36"/>
-        <v>940000</v>
+        <v>82500</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3775,7 +3828,7 @@
       </c>
       <c r="B146" s="24">
         <f>B33+(IF(0&gt;B144,-B144,-B33))</f>
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="C146" s="24">
         <f t="shared" ref="C146:D146" si="37">C33+(IF(0&gt;C144,-C144,-C33))</f>
@@ -3787,7 +3840,7 @@
       </c>
       <c r="E146" s="11">
         <f>SUM(B146:D146)</f>
-        <v>0</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3802,11 +3855,11 @@
       </c>
       <c r="D147" s="11">
         <f>-B146</f>
-        <v>0</v>
+        <v>-48000</v>
       </c>
       <c r="E147" s="11">
         <f t="shared" ref="E147:E148" si="38">SUM(B147:D147)</f>
-        <v>0</v>
+        <v>-48000</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3821,11 +3874,11 @@
       </c>
       <c r="D148" s="50">
         <f>D147*B39*(3/12)</f>
-        <v>0</v>
+        <v>-1920</v>
       </c>
       <c r="E148" s="11">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>-1920</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3834,7 +3887,7 @@
       </c>
       <c r="B149" s="68">
         <f>SUM(B146:B148)</f>
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="C149" s="68">
         <f t="shared" ref="C149:D149" si="39">SUM(C146:C148)</f>
@@ -3842,11 +3895,11 @@
       </c>
       <c r="D149" s="68">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>-49920</v>
       </c>
       <c r="E149" s="69">
         <f>SUM(E146:E148)</f>
-        <v>0</v>
+        <v>-1920</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3855,19 +3908,19 @@
       </c>
       <c r="B150" s="29">
         <f>B144+B149</f>
-        <v>170000</v>
+        <v>30000</v>
       </c>
       <c r="C150" s="29">
         <f t="shared" ref="C150:E150" si="40">C144+C149</f>
-        <v>580000</v>
+        <v>40000</v>
       </c>
       <c r="D150" s="29">
         <f t="shared" si="40"/>
-        <v>940000</v>
+        <v>80580</v>
       </c>
       <c r="E150" s="29">
         <f t="shared" si="40"/>
-        <v>940000</v>
+        <v>80580</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -3894,28 +3947,28 @@
       <c r="E153" s="4"/>
     </row>
     <row r="154" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="70" t="s">
+      <c r="A154" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="B154" s="70"/>
+      <c r="B154" s="71"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
     </row>
     <row r="155" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="70" t="s">
+      <c r="A155" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="B155" s="70"/>
+      <c r="B155" s="71"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
     </row>
     <row r="156" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="70" t="s">
+      <c r="A156" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="B156" s="70"/>
+      <c r="B156" s="71"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -3938,7 +3991,7 @@
       </c>
       <c r="B158" s="48">
         <f>ROUND(D115*E49,-3)</f>
-        <v>200000</v>
+        <v>499000</v>
       </c>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
@@ -3950,7 +4003,7 @@
       </c>
       <c r="B159" s="31">
         <f>B157-B158</f>
-        <v>800000</v>
+        <v>501000</v>
       </c>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
@@ -3962,7 +4015,7 @@
       </c>
       <c r="B160" s="61">
         <f>E127</f>
-        <v>0</v>
+        <v>260000</v>
       </c>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -3974,7 +4027,7 @@
       </c>
       <c r="B161" s="31">
         <f>B159-B160</f>
-        <v>800000</v>
+        <v>241000</v>
       </c>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
@@ -3986,7 +4039,7 @@
       </c>
       <c r="B162" s="61">
         <f>E148</f>
-        <v>0</v>
+        <v>-1920</v>
       </c>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
@@ -3998,7 +4051,7 @@
       </c>
       <c r="B163" s="33">
         <f>B161+B162</f>
-        <v>800000</v>
+        <v>239080</v>
       </c>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -4028,28 +4081,28 @@
       <c r="E166" s="4"/>
     </row>
     <row r="167" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="70" t="s">
+      <c r="A167" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="B167" s="70"/>
+      <c r="B167" s="71"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
     </row>
     <row r="168" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="70" t="s">
+      <c r="A168" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="B168" s="70"/>
+      <c r="B168" s="71"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
     </row>
     <row r="169" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="71" t="s">
+      <c r="A169" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="B169" s="71"/>
+      <c r="B169" s="72"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
@@ -4069,7 +4122,7 @@
       </c>
       <c r="B171" s="31">
         <f>E150</f>
-        <v>940000</v>
+        <v>80580</v>
       </c>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
@@ -4105,7 +4158,7 @@
       </c>
       <c r="B174" s="31">
         <f>D119</f>
-        <v>10000</v>
+        <v>24950</v>
       </c>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
@@ -4117,7 +4170,7 @@
       </c>
       <c r="B175" s="31">
         <f>B40</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
@@ -4129,7 +4182,7 @@
       </c>
       <c r="B176" s="61">
         <f>B43+B36+B37</f>
-        <v>0</v>
+        <v>367000</v>
       </c>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
@@ -4141,7 +4194,7 @@
       </c>
       <c r="B177" s="33">
         <f>SUM(B171:B176)</f>
-        <v>1044600</v>
+        <v>617130</v>
       </c>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
@@ -4169,7 +4222,7 @@
       </c>
       <c r="B180" s="42">
         <f>D79*B20</f>
-        <v>0</v>
+        <v>28400</v>
       </c>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
@@ -4181,7 +4234,7 @@
       </c>
       <c r="B181" s="31">
         <f>B41</f>
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
@@ -4193,7 +4246,7 @@
       </c>
       <c r="B182" s="31">
         <f>B42+B163-B34</f>
-        <v>800000</v>
+        <v>438730</v>
       </c>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
@@ -4205,7 +4258,7 @@
       </c>
       <c r="B183" s="40">
         <f>SUM(B180:B182)</f>
-        <v>800000</v>
+        <v>617130</v>
       </c>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
@@ -4214,12 +4267,6 @@
     <row r="184" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B69:E69"/>
     <mergeCell ref="A156:B156"/>
     <mergeCell ref="A167:B167"/>
     <mergeCell ref="A168:B168"/>
@@ -4230,6 +4277,12 @@
     <mergeCell ref="B131:E131"/>
     <mergeCell ref="A154:B154"/>
     <mergeCell ref="A155:B155"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B69:E69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>